<commit_message>
translated filler sentences, both scrambled and default in excel
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{921D24DE-9122-CD40-9FDC-D132660B9D4F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{36EC57A6-E75D-0E40-8540-5AA9459D1106}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13400" yWindow="460" windowWidth="19200" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8520" yWindow="460" windowWidth="24060" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
   <si>
     <t xml:space="preserve">sentence </t>
   </si>
@@ -319,13 +319,2213 @@
   </si>
   <si>
     <t>There are two girls who are wearing blue clothes</t>
+  </si>
+  <si>
+    <r>
+      <t>왼쪽에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>남자아이가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>축구공</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>네</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가지고</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>축구공</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>네</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가지고</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>남자가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>왼쪽에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>세</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>남자아이가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>공을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>찬다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>공을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>차는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>남자아이가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>세</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명이다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>남자아이가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>말</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>네</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>마리를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>타고</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>말</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>네마리를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>타는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아이가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>남자아이다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>여자아이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>네</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>토끼를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>얻었다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>토끼를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>얻은</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아이가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>네</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명이다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>네</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해적이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보물</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>옆에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>앉아있다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>보물</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>옆에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>앉아</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해적이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>네</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명이다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>제일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>왼쪽에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해적이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>물고기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>세마리를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>잡았다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>물고기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>세마리를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>잡은</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해적이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>제일</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>왼쪽에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>나무</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>세</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>그루에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>걸려있다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>등이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>걸려있는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>나무가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>세</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>그루다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>여자아이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>두</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>푸른색</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>옷을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>입고</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>푸른색</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>옷을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>입고</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>여자아이가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>두</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명이다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>남자아이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>세</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>공을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>찼다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>공을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>찬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>남자아이가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>세</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명이다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>토끼를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>얻은</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>여자아이가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>네</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명이다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>해적</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>네</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>명이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>보물</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>옆에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>앉아</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>있다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>세</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>그루의</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>나무에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>등이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>달려있다</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>등이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>달려있는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>나무는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>세</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>그루다</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -358,6 +2558,19 @@
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -368,13 +2581,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,14 +2604,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,12 +2902,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
     <col min="7" max="7" width="27.1640625" customWidth="1"/>
     <col min="15" max="15" width="17.33203125" customWidth="1"/>
   </cols>
@@ -712,20 +2934,20 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
       <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
       <c r="P2" t="s">
         <v>35</v>
       </c>
@@ -739,20 +2961,20 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
       <c r="P3" t="s">
         <v>36</v>
       </c>
@@ -766,20 +2988,20 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
       <c r="H4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
       <c r="P4" t="s">
         <v>37</v>
       </c>
@@ -793,20 +3015,20 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
       <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
       <c r="P5" t="s">
         <v>38</v>
       </c>
@@ -820,20 +3042,20 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
       <c r="H6" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
       <c r="P6" t="s">
         <v>39</v>
       </c>
@@ -847,20 +3069,20 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
       <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
       <c r="P7" t="s">
         <v>40</v>
       </c>
@@ -874,20 +3096,20 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
       <c r="H8" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
       <c r="P8" t="s">
         <v>41</v>
       </c>
@@ -901,20 +3123,20 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
       <c r="H9" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
       <c r="P9" t="s">
         <v>42</v>
       </c>
@@ -928,20 +3150,20 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
       <c r="H10" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
       <c r="P10" t="s">
         <v>43</v>
       </c>
@@ -955,20 +3177,20 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
       <c r="H11" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
       <c r="P11" t="s">
         <v>44</v>
       </c>
@@ -982,20 +3204,20 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
       <c r="H12" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
       <c r="P12" t="s">
         <v>45</v>
       </c>
@@ -1009,20 +3231,20 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
       <c r="H13" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
       <c r="P13" t="s">
         <v>46</v>
       </c>
@@ -1036,20 +3258,20 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
       <c r="H14" t="s">
         <v>31</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
       <c r="P14" t="s">
         <v>47</v>
       </c>
@@ -1063,20 +3285,20 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
       <c r="H15" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
       <c r="P15" t="s">
         <v>48</v>
       </c>
@@ -1090,20 +3312,20 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
       <c r="H16" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
       <c r="P16" t="s">
         <v>49</v>
       </c>
@@ -1117,20 +3339,20 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
       <c r="H17" t="s">
         <v>34</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
       <c r="P17" t="s">
         <v>50</v>
       </c>
@@ -1140,70 +3362,213 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" ht="17">
       <c r="B20" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="E20" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="L20" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" ht="17">
       <c r="B21" s="4" t="s">
         <v>86</v>
       </c>
+      <c r="E21" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="L21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" ht="17">
       <c r="B22" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="E22" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="L22" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" ht="17">
       <c r="B23" s="4" t="s">
         <v>87</v>
       </c>
+      <c r="E23" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="L23" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" ht="17">
       <c r="B24" s="4" t="s">
         <v>88</v>
       </c>
+      <c r="E24" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="L24" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" ht="17">
       <c r="B25" s="4" t="s">
         <v>89</v>
       </c>
+      <c r="E25" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="L25" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" ht="17">
       <c r="B26" s="4" t="s">
         <v>90</v>
       </c>
+      <c r="E26" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="L26" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" ht="17">
       <c r="B27" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="E27" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="L27" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" ht="17">
       <c r="B28" s="4" t="s">
         <v>92</v>
       </c>
+      <c r="E28" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="L28" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" ht="17">
       <c r="B29" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="E29" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="L29" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" ht="17">
       <c r="B30" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="E30" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="L30" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" ht="17">
       <c r="B31" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="E31" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="L31" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" ht="17">
       <c r="B32" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="E32" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="L32" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
attached all audio files for fillers and edited java for fillers
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{36EC57A6-E75D-0E40-8540-5AA9459D1106}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4E95991F-83CF-F94C-A57D-6BBFD5D57B9D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="460" windowWidth="24060" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1580" yWindow="460" windowWidth="27080" windowHeight="19100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2902,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3363,6 +3363,9 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="17">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
       <c r="B20" s="4" t="s">
         <v>84</v>
       </c>
@@ -3379,6 +3382,9 @@
       <c r="O20" s="8"/>
     </row>
     <row r="21" spans="1:16" ht="17">
+      <c r="A21" s="4">
+        <v>2</v>
+      </c>
       <c r="B21" s="4" t="s">
         <v>86</v>
       </c>
@@ -3395,6 +3401,9 @@
       <c r="O21" s="8"/>
     </row>
     <row r="22" spans="1:16" ht="17">
+      <c r="A22" s="4">
+        <v>3</v>
+      </c>
       <c r="B22" s="4" t="s">
         <v>85</v>
       </c>
@@ -3411,6 +3420,9 @@
       <c r="O22" s="8"/>
     </row>
     <row r="23" spans="1:16" ht="17">
+      <c r="A23" s="4">
+        <v>4</v>
+      </c>
       <c r="B23" s="4" t="s">
         <v>87</v>
       </c>
@@ -3427,6 +3439,9 @@
       <c r="O23" s="8"/>
     </row>
     <row r="24" spans="1:16" ht="17">
+      <c r="A24" s="4">
+        <v>5</v>
+      </c>
       <c r="B24" s="4" t="s">
         <v>88</v>
       </c>
@@ -3443,6 +3458,9 @@
       <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:16" ht="17">
+      <c r="A25" s="4">
+        <v>6</v>
+      </c>
       <c r="B25" s="4" t="s">
         <v>89</v>
       </c>
@@ -3459,6 +3477,9 @@
       <c r="O25" s="8"/>
     </row>
     <row r="26" spans="1:16" ht="17">
+      <c r="A26" s="4">
+        <v>7</v>
+      </c>
       <c r="B26" s="4" t="s">
         <v>90</v>
       </c>
@@ -3475,6 +3496,9 @@
       <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:16" ht="17">
+      <c r="A27" s="4">
+        <v>8</v>
+      </c>
       <c r="B27" s="4" t="s">
         <v>91</v>
       </c>
@@ -3491,6 +3515,9 @@
       <c r="O27" s="8"/>
     </row>
     <row r="28" spans="1:16" ht="17">
+      <c r="A28" s="4">
+        <v>9</v>
+      </c>
       <c r="B28" s="4" t="s">
         <v>92</v>
       </c>
@@ -3507,6 +3534,9 @@
       <c r="O28" s="8"/>
     </row>
     <row r="29" spans="1:16" ht="17">
+      <c r="A29" s="4">
+        <v>10</v>
+      </c>
       <c r="B29" s="4" t="s">
         <v>93</v>
       </c>
@@ -3523,6 +3553,9 @@
       <c r="O29" s="8"/>
     </row>
     <row r="30" spans="1:16" ht="17">
+      <c r="A30" s="4">
+        <v>11</v>
+      </c>
       <c r="B30" s="4" t="s">
         <v>94</v>
       </c>
@@ -3539,6 +3572,9 @@
       <c r="O30" s="8"/>
     </row>
     <row r="31" spans="1:16" ht="17">
+      <c r="A31" s="4">
+        <v>12</v>
+      </c>
       <c r="B31" s="4" t="s">
         <v>95</v>
       </c>
@@ -3555,6 +3591,9 @@
       <c r="O31" s="8"/>
     </row>
     <row r="32" spans="1:16" ht="17">
+      <c r="A32" s="4">
+        <v>13</v>
+      </c>
       <c r="B32" s="4" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
recorded audio with translations using "enu" for "every"
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BC5DF27A-53FE-9A4D-BB5E-3BB725653E23}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{57A288AD-31A7-864B-8F15-89A3CE8966D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="27080" windowHeight="19100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="151">
   <si>
     <t xml:space="preserve">sentence </t>
   </si>
@@ -2519,6 +2519,102 @@
       </rPr>
       <t>명이다</t>
     </r>
+  </si>
+  <si>
+    <t>어느 해적이나 통 하나에 기대어 있다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 어느 통에나 기대어 있다</t>
+  </si>
+  <si>
+    <t xml:space="preserve">어느 해적이나 물고기 한마리를 잡았다 </t>
+  </si>
+  <si>
+    <t>해적 한사람이 어느 물고기나 잡았다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 어느 낚시대나 잡고 있다</t>
+  </si>
+  <si>
+    <t>어느 해적이나 상어 한마리를 먹였다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 어느 상어나 먹였다</t>
+  </si>
+  <si>
+    <t>어느 해적이나 병 하나를 잡고 있다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 어느 병이나 잡고 있다</t>
+  </si>
+  <si>
+    <t>어느 상어나 물고기 한마리를 물고 있다</t>
+  </si>
+  <si>
+    <t>상어 한마리가 어느 물고기나 물고 있다</t>
+  </si>
+  <si>
+    <t>어느 상어나 해적 한사람을 공격했다</t>
+  </si>
+  <si>
+    <t>상어 한마리가 어느 해적이나 공격했다</t>
+  </si>
+  <si>
+    <t>어느 여자아이나 강아지 한마리를 쓰다듬고 있다</t>
+  </si>
+  <si>
+    <t>여자아이 하나가 어느 강아지나 쓰다듬었다</t>
+  </si>
+  <si>
+    <t>통 하나에 어느 해적이나 기대어 있다</t>
+  </si>
+  <si>
+    <t>물고기 한마리를 어느 해적이나  잡았다</t>
+  </si>
+  <si>
+    <t>어느 물고기이나 해적 한사람이 잡았다</t>
+  </si>
+  <si>
+    <t>낚시대 하나를 어느 해적이나 잡고 있다</t>
+  </si>
+  <si>
+    <t>어느 낚시대나 해적 한사람이 잡고 있다</t>
+  </si>
+  <si>
+    <t>상어 한마리를 어느 해적이나 먹였다</t>
+  </si>
+  <si>
+    <t>어느 상어나 해적 한사람이 먹였다</t>
+  </si>
+  <si>
+    <t>병 하나를 어느 해적이나 잡고 있다</t>
+  </si>
+  <si>
+    <t>어느 병이나 해적 한사람이 잡고 있다</t>
+  </si>
+  <si>
+    <t>물고기 한마리를 어느 상어나 물고 있다</t>
+  </si>
+  <si>
+    <t>어느 물고기나 상어 한마리가 물고 있다</t>
+  </si>
+  <si>
+    <t>해적 한사람을 어느 상어나 공격했다</t>
+  </si>
+  <si>
+    <t>어느 해적이나 상어 한마리가 공격했다</t>
+  </si>
+  <si>
+    <t>강아지 한마리를 어느 여자아이나 쓰다듬고 있다</t>
+  </si>
+  <si>
+    <t>어느 강아지나 여자아이 하나가 쓰다듬었다</t>
+  </si>
+  <si>
+    <t>어느 해적이나 낚시대 하나를 잡고 있다</t>
+  </si>
+  <si>
+    <t>어느 통에나 해적 한사람이 기대어 있다</t>
   </si>
 </sst>
 </file>
@@ -2572,7 +2668,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2591,6 +2687,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2604,7 +2712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2621,6 +2729,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2901,10 +3011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="170" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="D27" zoomScale="150" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3714,6 +3824,450 @@
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
     </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="E34" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="4">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" t="s">
+        <v>19</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="4">
+        <v>1</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="4">
+        <v>2</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="4">
+        <v>2</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" t="s">
+        <v>22</v>
+      </c>
+      <c r="L38" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" s="4">
+        <v>3</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" t="s">
+        <v>23</v>
+      </c>
+      <c r="L39" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" s="4">
+        <v>3</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" t="s">
+        <v>24</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="4">
+        <v>4</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" t="s">
+        <v>25</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" s="4">
+        <v>4</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" t="s">
+        <v>26</v>
+      </c>
+      <c r="L42" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="4">
+        <v>5</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L43" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="4">
+        <v>5</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" t="s">
+        <v>28</v>
+      </c>
+      <c r="L44" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="13"/>
+      <c r="P44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="4">
+        <v>6</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" t="s">
+        <v>29</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="13"/>
+      <c r="P45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="4">
+        <v>6</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" t="s">
+        <v>30</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="13"/>
+      <c r="P46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="4">
+        <v>7</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" t="s">
+        <v>31</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="13"/>
+      <c r="P47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="4">
+        <v>7</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="4"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" t="s">
+        <v>32</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="13"/>
+      <c r="P48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="4">
+        <v>8</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" t="s">
+        <v>33</v>
+      </c>
+      <c r="L49" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="13"/>
+      <c r="P49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" s="4">
+        <v>8</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" t="s">
+        <v>34</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+      <c r="P50" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
renamed audio recordings and under folder "enu" recordings
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{57A288AD-31A7-864B-8F15-89A3CE8966D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A8CD6C45-B286-9847-9927-AC8FAFC36722}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6860" yWindow="460" windowWidth="27080" windowHeight="19100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
updated excel sheet with korean translations using "enu"
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A8CD6C45-B286-9847-9927-AC8FAFC36722}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{784D5F70-0476-464F-942C-C3A7A63F98CC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="460" windowWidth="27080" windowHeight="19100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7380" yWindow="560" windowWidth="21240" windowHeight="13420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3013,8 +3013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D27" zoomScale="150" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="91" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3469,804 +3469,804 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="18">
+      <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="4">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="7">
-        <v>53</v>
-      </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-    </row>
-    <row r="21" spans="1:16" ht="18">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="4">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="7">
-        <v>63</v>
-      </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-    </row>
-    <row r="22" spans="1:16" ht="18">
+      <c r="C21" s="4"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="4">
+        <v>2</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="7">
-        <v>63</v>
-      </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-    </row>
-    <row r="23" spans="1:16" ht="18">
+      <c r="C22" s="4"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="4">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="7">
-        <v>75</v>
-      </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-    </row>
-    <row r="24" spans="1:16" ht="18">
+      <c r="C23" s="4"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="4">
+        <v>3</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="7">
-        <v>56</v>
-      </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-    </row>
-    <row r="25" spans="1:16" ht="18">
+      <c r="C24" s="4"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="4">
+        <v>3</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="7">
-        <v>56</v>
-      </c>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-    </row>
-    <row r="26" spans="1:16" ht="18">
+      <c r="C25" s="4"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="4">
+        <v>4</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="7">
+      <c r="C26" s="4"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="4">
+        <v>4</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="4">
+        <v>5</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-    </row>
-    <row r="27" spans="1:16" ht="18">
-      <c r="A27" s="4">
+      <c r="C28" s="4"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="4">
+        <v>5</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="4">
+        <v>6</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" t="s">
+        <v>29</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="4">
+        <v>6</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" t="s">
+        <v>30</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="4">
+        <v>7</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" t="s">
+        <v>31</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="4">
+        <v>7</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" t="s">
+        <v>32</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="4">
         <v>8</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="7">
-        <v>9</v>
-      </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-    </row>
-    <row r="28" spans="1:16" ht="18">
-      <c r="A28" s="4">
-        <v>9</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7">
+      <c r="B34" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-    </row>
-    <row r="29" spans="1:16" ht="18">
-      <c r="A29" s="4">
-        <v>10</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="7">
-        <v>5</v>
-      </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-    </row>
-    <row r="30" spans="1:16" ht="18">
-      <c r="A30" s="4">
-        <v>11</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7">
-        <v>5</v>
-      </c>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-    </row>
-    <row r="31" spans="1:16" ht="18">
-      <c r="A31" s="4">
-        <v>12</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="7">
-        <v>54</v>
-      </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-    </row>
-    <row r="32" spans="1:16" ht="18">
-      <c r="A32" s="4">
-        <v>13</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="7">
-        <v>54</v>
-      </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-    </row>
-    <row r="34" spans="1:16">
-      <c r="A34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="C34" s="4"/>
-      <c r="E34" s="1" t="s">
-        <v>18</v>
+      <c r="D34" s="2"/>
+      <c r="E34" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" t="s">
+        <v>33</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="2"/>
       <c r="E35" s="12" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="L35" s="13" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
       <c r="P35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
-      <c r="A36" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="18">
+      <c r="A38" s="4">
         <v>1</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B38" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="7">
+        <v>53</v>
+      </c>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+    </row>
+    <row r="39" spans="1:16" ht="18">
+      <c r="A39" s="4">
         <v>2</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16">
-      <c r="A37" s="4">
-        <v>2</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" t="s">
-        <v>21</v>
-      </c>
-      <c r="L37" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
-      <c r="A38" s="4">
-        <v>2</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" t="s">
-        <v>22</v>
-      </c>
-      <c r="L38" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16">
-      <c r="A39" s="4">
-        <v>3</v>
-      </c>
       <c r="B39" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" t="s">
-        <v>23</v>
-      </c>
-      <c r="L39" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
-      <c r="P39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16">
+        <v>86</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="7">
+        <v>63</v>
+      </c>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+    </row>
+    <row r="40" spans="1:16" ht="18">
       <c r="A40" s="4">
         <v>3</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" t="s">
-        <v>24</v>
-      </c>
-      <c r="L40" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
-      <c r="P40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16">
+        <v>85</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="7">
+        <v>63</v>
+      </c>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+    </row>
+    <row r="41" spans="1:16" ht="18">
       <c r="A41" s="4">
         <v>4</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="7">
+        <v>75</v>
+      </c>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+    </row>
+    <row r="42" spans="1:16" ht="18">
+      <c r="A42" s="4">
+        <v>5</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="7">
+        <v>56</v>
+      </c>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+    </row>
+    <row r="43" spans="1:16" ht="18">
+      <c r="A43" s="4">
+        <v>6</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="7">
+        <v>56</v>
+      </c>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+    </row>
+    <row r="44" spans="1:16" ht="18">
+      <c r="A44" s="4">
         <v>7</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" t="s">
-        <v>25</v>
-      </c>
-      <c r="L41" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16">
-      <c r="A42" s="4">
-        <v>4</v>
-      </c>
-      <c r="B42" s="4" t="s">
+      <c r="B44" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="7">
+        <v>9</v>
+      </c>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+    </row>
+    <row r="45" spans="1:16" ht="18">
+      <c r="A45" s="4">
         <v>8</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" t="s">
-        <v>26</v>
-      </c>
-      <c r="L42" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16">
-      <c r="A43" s="4">
+      <c r="B45" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="7">
+        <v>9</v>
+      </c>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+    </row>
+    <row r="46" spans="1:16" ht="18">
+      <c r="A46" s="4">
+        <v>9</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="7">
+        <v>16</v>
+      </c>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+    </row>
+    <row r="47" spans="1:16" ht="18">
+      <c r="A47" s="4">
+        <v>10</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="7">
         <v>5</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" t="s">
-        <v>27</v>
-      </c>
-      <c r="L43" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="13"/>
-      <c r="P43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16">
-      <c r="A44" s="4">
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+    </row>
+    <row r="48" spans="1:16" ht="18">
+      <c r="A48" s="4">
+        <v>11</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="7">
         <v>5</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" t="s">
-        <v>28</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="13"/>
-      <c r="P44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
-      <c r="A45" s="4">
-        <v>6</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" t="s">
-        <v>29</v>
-      </c>
-      <c r="L45" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="13"/>
-      <c r="P45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16">
-      <c r="A46" s="4">
-        <v>6</v>
-      </c>
-      <c r="B46" s="4" t="s">
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+    </row>
+    <row r="49" spans="1:15" ht="18">
+      <c r="A49" s="4">
         <v>12</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" t="s">
-        <v>30</v>
-      </c>
-      <c r="L46" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="13"/>
-      <c r="P46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16">
-      <c r="A47" s="4">
-        <v>7</v>
-      </c>
-      <c r="B47" s="4" t="s">
+      <c r="B49" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="7">
+        <v>54</v>
+      </c>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10"/>
+    </row>
+    <row r="50" spans="1:15" ht="18">
+      <c r="A50" s="4">
         <v>13</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" t="s">
-        <v>31</v>
-      </c>
-      <c r="L47" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="13"/>
-      <c r="P47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="A48" s="4">
-        <v>7</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" t="s">
-        <v>32</v>
-      </c>
-      <c r="L48" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="M48" s="13"/>
-      <c r="N48" s="13"/>
-      <c r="O48" s="13"/>
-      <c r="P48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16">
-      <c r="A49" s="4">
-        <v>8</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" t="s">
-        <v>33</v>
-      </c>
-      <c r="L49" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="M49" s="13"/>
-      <c r="N49" s="13"/>
-      <c r="O49" s="13"/>
-      <c r="P49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16">
-      <c r="A50" s="4">
-        <v>8</v>
-      </c>
       <c r="B50" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" t="s">
-        <v>34</v>
-      </c>
-      <c r="L50" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-      <c r="P50" t="s">
-        <v>50</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="7">
+        <v>54</v>
+      </c>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added email list info
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/git/korean_scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{784D5F70-0476-464F-942C-C3A7A63F98CC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="560" windowWidth="21240" windowHeight="13420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7380" yWindow="560" windowWidth="29680" windowHeight="20520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="154">
   <si>
     <t xml:space="preserve">sentence </t>
   </si>
@@ -2615,13 +2614,22 @@
   </si>
   <si>
     <t>어느 통에나 해적 한사람이 기대어 있다</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>list</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3010,1263 +3018,1344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="91" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:O50"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="116" zoomScalePageLayoutView="116" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="29.5" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.5" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="4"/>
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
-      <c r="P2" t="s">
+      <c r="P2" s="5"/>
+      <c r="Q2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
-      <c r="P3" t="s">
+      <c r="P3" s="5"/>
+      <c r="Q3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" t="s">
+      <c r="P4" s="5"/>
+      <c r="Q4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" t="s">
+      <c r="P5" s="5"/>
+      <c r="Q5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" t="s">
+      <c r="P6" s="5"/>
+      <c r="Q6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" t="s">
+      <c r="P7" s="5"/>
+      <c r="Q7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-      <c r="P8" t="s">
+      <c r="P8" s="5"/>
+      <c r="Q8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" t="s">
+      <c r="P9" s="5"/>
+      <c r="Q9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" t="s">
+      <c r="H10" s="6"/>
+      <c r="I10" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" t="s">
+      <c r="P10" s="5"/>
+      <c r="Q10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="6" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" t="s">
+      <c r="H11" s="6"/>
+      <c r="I11" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-      <c r="P11" t="s">
+      <c r="P11" s="5"/>
+      <c r="Q11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" t="s">
+      <c r="H12" s="6"/>
+      <c r="I12" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-      <c r="P12" t="s">
+      <c r="P12" s="5"/>
+      <c r="Q12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" t="s">
+      <c r="H13" s="6"/>
+      <c r="I13" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
-      <c r="P13" t="s">
+      <c r="P13" s="5"/>
+      <c r="Q13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="6" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" t="s">
+      <c r="H14" s="6"/>
+      <c r="I14" t="s">
         <v>31</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-      <c r="P14" t="s">
+      <c r="P14" s="5"/>
+      <c r="Q14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" t="s">
+      <c r="H15" s="6"/>
+      <c r="I15" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="M15" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-      <c r="P15" t="s">
+      <c r="P15" s="5"/>
+      <c r="Q15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="6" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" t="s">
+      <c r="H16" s="6"/>
+      <c r="I16" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="M16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-      <c r="P16" t="s">
+      <c r="P16" s="5"/>
+      <c r="Q16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>8</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="6" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" t="s">
+      <c r="H17" s="6"/>
+      <c r="I17" t="s">
         <v>34</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
-      <c r="P17" t="s">
+      <c r="P17" s="5"/>
+      <c r="Q17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="E19" s="1" t="s">
+      <c r="D19" s="4"/>
+      <c r="F19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>1</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="12" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="12"/>
       <c r="G20" s="12"/>
-      <c r="H20" t="s">
+      <c r="H20" s="12"/>
+      <c r="I20" t="s">
         <v>19</v>
       </c>
-      <c r="L20" s="13" t="s">
+      <c r="M20" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="M20" s="13"/>
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
-      <c r="P20" t="s">
+      <c r="P20" s="13"/>
+      <c r="Q20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>1</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="12" t="s">
+      <c r="D21" s="4"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-      <c r="H21" t="s">
+      <c r="H21" s="12"/>
+      <c r="I21" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="M21" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="M21" s="13"/>
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
-      <c r="P21" t="s">
+      <c r="P21" s="13"/>
+      <c r="Q21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>2</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="12" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="12"/>
       <c r="G22" s="12"/>
-      <c r="H22" t="s">
+      <c r="H22" s="12"/>
+      <c r="I22" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="13" t="s">
+      <c r="M22" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="M22" s="13"/>
       <c r="N22" s="13"/>
       <c r="O22" s="13"/>
-      <c r="P22" t="s">
+      <c r="P22" s="13"/>
+      <c r="Q22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>2</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="12" t="s">
+      <c r="D23" s="4"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F23" s="12"/>
       <c r="G23" s="12"/>
-      <c r="H23" t="s">
+      <c r="H23" s="12"/>
+      <c r="I23" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="13" t="s">
+      <c r="M23" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="M23" s="13"/>
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
-      <c r="P23" t="s">
+      <c r="P23" s="13"/>
+      <c r="Q23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>3</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="12" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="F24" s="12"/>
       <c r="G24" s="12"/>
-      <c r="H24" t="s">
+      <c r="H24" s="12"/>
+      <c r="I24" t="s">
         <v>23</v>
       </c>
-      <c r="L24" s="13" t="s">
+      <c r="M24" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="M24" s="13"/>
       <c r="N24" s="13"/>
       <c r="O24" s="13"/>
-      <c r="P24" t="s">
+      <c r="P24" s="13"/>
+      <c r="Q24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>3</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="12" t="s">
+      <c r="D25" s="4"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="F25" s="12"/>
       <c r="G25" s="12"/>
-      <c r="H25" t="s">
+      <c r="H25" s="12"/>
+      <c r="I25" t="s">
         <v>24</v>
       </c>
-      <c r="L25" s="13" t="s">
+      <c r="M25" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="M25" s="13"/>
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
-      <c r="P25" t="s">
+      <c r="P25" s="13"/>
+      <c r="Q25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>4</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="12" t="s">
+      <c r="D26" s="4"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F26" s="12"/>
       <c r="G26" s="12"/>
-      <c r="H26" t="s">
+      <c r="H26" s="12"/>
+      <c r="I26" t="s">
         <v>25</v>
       </c>
-      <c r="L26" s="13" t="s">
+      <c r="M26" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="M26" s="13"/>
       <c r="N26" s="13"/>
       <c r="O26" s="13"/>
-      <c r="P26" t="s">
+      <c r="P26" s="13"/>
+      <c r="Q26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>4</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="12" t="s">
+      <c r="D27" s="4"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="F27" s="12"/>
       <c r="G27" s="12"/>
-      <c r="H27" t="s">
+      <c r="H27" s="12"/>
+      <c r="I27" t="s">
         <v>26</v>
       </c>
-      <c r="L27" s="13" t="s">
+      <c r="M27" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="M27" s="13"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
-      <c r="P27" t="s">
+      <c r="P27" s="13"/>
+      <c r="Q27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>5</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="12" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="F28" s="12"/>
       <c r="G28" s="12"/>
-      <c r="H28" t="s">
+      <c r="H28" s="12"/>
+      <c r="I28" t="s">
         <v>27</v>
       </c>
-      <c r="L28" s="13" t="s">
+      <c r="M28" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="M28" s="13"/>
       <c r="N28" s="13"/>
       <c r="O28" s="13"/>
-      <c r="P28" t="s">
+      <c r="P28" s="13"/>
+      <c r="Q28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>5</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="12" t="s">
+      <c r="D29" s="4"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="F29" s="12"/>
       <c r="G29" s="12"/>
-      <c r="H29" t="s">
+      <c r="H29" s="12"/>
+      <c r="I29" t="s">
         <v>28</v>
       </c>
-      <c r="L29" s="13" t="s">
+      <c r="M29" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="M29" s="13"/>
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
-      <c r="P29" t="s">
+      <c r="P29" s="13"/>
+      <c r="Q29" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>6</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="12" t="s">
+      <c r="D30" s="4"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="F30" s="12"/>
       <c r="G30" s="12"/>
-      <c r="H30" t="s">
+      <c r="H30" s="12"/>
+      <c r="I30" t="s">
         <v>29</v>
       </c>
-      <c r="L30" s="13" t="s">
+      <c r="M30" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="M30" s="13"/>
       <c r="N30" s="13"/>
       <c r="O30" s="13"/>
-      <c r="P30" t="s">
+      <c r="P30" s="13"/>
+      <c r="Q30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>6</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="12" t="s">
+      <c r="D31" s="4"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="F31" s="12"/>
       <c r="G31" s="12"/>
-      <c r="H31" t="s">
+      <c r="H31" s="12"/>
+      <c r="I31" t="s">
         <v>30</v>
       </c>
-      <c r="L31" s="13" t="s">
+      <c r="M31" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="M31" s="13"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
-      <c r="P31" t="s">
+      <c r="P31" s="13"/>
+      <c r="Q31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>7</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="12" t="s">
+      <c r="D32" s="4"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="F32" s="12"/>
       <c r="G32" s="12"/>
-      <c r="H32" t="s">
+      <c r="H32" s="12"/>
+      <c r="I32" t="s">
         <v>31</v>
       </c>
-      <c r="L32" s="13" t="s">
+      <c r="M32" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="M32" s="13"/>
       <c r="N32" s="13"/>
       <c r="O32" s="13"/>
-      <c r="P32" t="s">
+      <c r="P32" s="13"/>
+      <c r="Q32" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>7</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="12" t="s">
+      <c r="D33" s="4"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="F33" s="12"/>
       <c r="G33" s="12"/>
-      <c r="H33" t="s">
+      <c r="H33" s="12"/>
+      <c r="I33" t="s">
         <v>32</v>
       </c>
-      <c r="L33" s="13" t="s">
+      <c r="M33" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="M33" s="13"/>
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
-      <c r="P33" t="s">
+      <c r="P33" s="13"/>
+      <c r="Q33" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>8</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="12" t="s">
+      <c r="D34" s="4"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F34" s="12"/>
       <c r="G34" s="12"/>
-      <c r="H34" t="s">
+      <c r="H34" s="12"/>
+      <c r="I34" t="s">
         <v>33</v>
       </c>
-      <c r="L34" s="13" t="s">
+      <c r="M34" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="M34" s="13"/>
       <c r="N34" s="13"/>
       <c r="O34" s="13"/>
-      <c r="P34" t="s">
+      <c r="P34" s="13"/>
+      <c r="Q34" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>8</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="12" t="s">
+      <c r="D35" s="4"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="F35" s="12"/>
       <c r="G35" s="12"/>
-      <c r="H35" t="s">
+      <c r="H35" s="12"/>
+      <c r="I35" t="s">
         <v>34</v>
       </c>
-      <c r="L35" s="13" t="s">
+      <c r="M35" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="M35" s="13"/>
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
-      <c r="P35" t="s">
+      <c r="P35" s="13"/>
+      <c r="Q35" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="18">
+    <row r="38" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>1</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="7"/>
       <c r="D38" s="7"/>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="7"/>
+      <c r="F38" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="7">
+      <c r="H38" s="6"/>
+      <c r="I38" s="7">
         <v>53</v>
       </c>
-      <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
-      <c r="L38" s="9" t="s">
+      <c r="L38" s="7"/>
+      <c r="M38" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="M38" s="10"/>
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
-    </row>
-    <row r="39" spans="1:16" ht="18">
+      <c r="P38" s="10"/>
+    </row>
+    <row r="39" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>2</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="7"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="7"/>
+      <c r="F39" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="7">
+      <c r="H39" s="6"/>
+      <c r="I39" s="7">
         <v>63</v>
       </c>
-      <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
-      <c r="L39" s="9" t="s">
+      <c r="L39" s="7"/>
+      <c r="M39" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="M39" s="10"/>
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
-    </row>
-    <row r="40" spans="1:16" ht="18">
+      <c r="P39" s="10"/>
+    </row>
+    <row r="40" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>3</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="7"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="8" t="s">
+      <c r="E40" s="7"/>
+      <c r="F40" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="7">
+      <c r="H40" s="6"/>
+      <c r="I40" s="7">
         <v>63</v>
       </c>
-      <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
-      <c r="L40" s="9" t="s">
+      <c r="L40" s="7"/>
+      <c r="M40" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="M40" s="10"/>
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
-    </row>
-    <row r="41" spans="1:16" ht="18">
+      <c r="P40" s="10"/>
+    </row>
+    <row r="41" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>4</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="7"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="8" t="s">
+      <c r="E41" s="7"/>
+      <c r="F41" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="7">
+      <c r="H41" s="6"/>
+      <c r="I41" s="7">
         <v>75</v>
       </c>
-      <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
-      <c r="L41" s="11" t="s">
+      <c r="L41" s="7"/>
+      <c r="M41" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="M41" s="10"/>
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
-    </row>
-    <row r="42" spans="1:16" ht="18">
+      <c r="P41" s="10"/>
+    </row>
+    <row r="42" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>5</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="7"/>
       <c r="D42" s="7"/>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="7"/>
+      <c r="F42" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F42" s="6"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="7">
+      <c r="H42" s="6"/>
+      <c r="I42" s="7">
         <v>56</v>
       </c>
-      <c r="I42" s="7"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
-      <c r="L42" s="9" t="s">
+      <c r="L42" s="7"/>
+      <c r="M42" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="M42" s="10"/>
       <c r="N42" s="10"/>
       <c r="O42" s="10"/>
-    </row>
-    <row r="43" spans="1:16" ht="18">
+      <c r="P42" s="10"/>
+    </row>
+    <row r="43" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>6</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="4"/>
+      <c r="C43" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="7"/>
       <c r="D43" s="7"/>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="7"/>
+      <c r="F43" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="7">
+      <c r="H43" s="6"/>
+      <c r="I43" s="7">
         <v>56</v>
       </c>
-      <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
-      <c r="L43" s="9" t="s">
+      <c r="L43" s="7"/>
+      <c r="M43" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="M43" s="10"/>
       <c r="N43" s="10"/>
       <c r="O43" s="10"/>
-    </row>
-    <row r="44" spans="1:16" ht="18">
+      <c r="P43" s="10"/>
+    </row>
+    <row r="44" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>7</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="4"/>
+      <c r="C44" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="7"/>
       <c r="D44" s="7"/>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="7"/>
+      <c r="F44" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="7">
+      <c r="H44" s="6"/>
+      <c r="I44" s="7">
         <v>9</v>
       </c>
-      <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
-      <c r="L44" s="9" t="s">
+      <c r="L44" s="7"/>
+      <c r="M44" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="M44" s="10"/>
       <c r="N44" s="10"/>
       <c r="O44" s="10"/>
-    </row>
-    <row r="45" spans="1:16" ht="18">
+      <c r="P44" s="10"/>
+    </row>
+    <row r="45" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>8</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="7"/>
       <c r="D45" s="7"/>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="7"/>
+      <c r="F45" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="7">
+      <c r="H45" s="6"/>
+      <c r="I45" s="7">
         <v>9</v>
       </c>
-      <c r="I45" s="7"/>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
-      <c r="L45" s="9" t="s">
+      <c r="L45" s="7"/>
+      <c r="M45" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="M45" s="10"/>
       <c r="N45" s="10"/>
       <c r="O45" s="10"/>
-    </row>
-    <row r="46" spans="1:16" ht="18">
+      <c r="P45" s="10"/>
+    </row>
+    <row r="46" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>9</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="4"/>
+      <c r="C46" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C46" s="7"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="7"/>
+      <c r="F46" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="7">
+      <c r="H46" s="6"/>
+      <c r="I46" s="7">
         <v>16</v>
       </c>
-      <c r="I46" s="7"/>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
-      <c r="L46" s="9" t="s">
+      <c r="L46" s="7"/>
+      <c r="M46" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="M46" s="10"/>
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
-    </row>
-    <row r="47" spans="1:16" ht="18">
+      <c r="P46" s="10"/>
+    </row>
+    <row r="47" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>10</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="4"/>
+      <c r="C47" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C47" s="7"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="7"/>
+      <c r="F47" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="7">
+      <c r="H47" s="6"/>
+      <c r="I47" s="7">
         <v>5</v>
       </c>
-      <c r="I47" s="7"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
-      <c r="L47" s="9" t="s">
+      <c r="L47" s="7"/>
+      <c r="M47" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="M47" s="10"/>
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
-    </row>
-    <row r="48" spans="1:16" ht="18">
+      <c r="P47" s="10"/>
+    </row>
+    <row r="48" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>11</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C48" s="7"/>
       <c r="D48" s="7"/>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="7"/>
+      <c r="F48" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="7">
+      <c r="H48" s="6"/>
+      <c r="I48" s="7">
         <v>5</v>
       </c>
-      <c r="I48" s="7"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
-      <c r="L48" s="9" t="s">
+      <c r="L48" s="7"/>
+      <c r="M48" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="M48" s="10"/>
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
-    </row>
-    <row r="49" spans="1:15" ht="18">
+      <c r="P48" s="10"/>
+    </row>
+    <row r="49" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>12</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="4"/>
+      <c r="C49" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="7"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="8" t="s">
+      <c r="E49" s="7"/>
+      <c r="F49" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="F49" s="6"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="7">
+      <c r="H49" s="6"/>
+      <c r="I49" s="7">
         <v>54</v>
       </c>
-      <c r="I49" s="7"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
-      <c r="L49" s="9" t="s">
+      <c r="L49" s="7"/>
+      <c r="M49" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="M49" s="10"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
-    </row>
-    <row r="50" spans="1:15" ht="18">
+      <c r="P49" s="10"/>
+    </row>
+    <row r="50" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>13</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="4"/>
+      <c r="C50" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="7"/>
       <c r="D50" s="7"/>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="7"/>
+      <c r="F50" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="7">
+      <c r="H50" s="6"/>
+      <c r="I50" s="7">
         <v>54</v>
       </c>
-      <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
-      <c r="L50" s="9" t="s">
+      <c r="L50" s="7"/>
+      <c r="M50" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="M50" s="10"/>
       <c r="N50" s="10"/>
       <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added all results of translations on Excel sheet
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/git/korean_scope/experiments/experigen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A1FFCCF8-EB2D-E44E-9366-F7D8CDAE2E16}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15300" yWindow="980" windowWidth="29680" windowHeight="20520" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4920" yWindow="460" windowWidth="27820" windowHeight="19980" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="all sentences" sheetId="1" r:id="rId1"/>
+    <sheet name="randomized" sheetId="2" r:id="rId2"/>
     <sheet name="email sentences" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="results" sheetId="4" r:id="rId4"/>
+    <sheet name="data" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="292">
   <si>
     <t xml:space="preserve">sentence </t>
   </si>
@@ -2653,13 +2655,885 @@
   </si>
   <si>
     <t>Batch 2</t>
+  </si>
+  <si>
+    <t>participant 1</t>
+  </si>
+  <si>
+    <t>All sharks attacked one person.</t>
+  </si>
+  <si>
+    <t>One girl taps a dog.</t>
+  </si>
+  <si>
+    <t>All pirates hold one fishing pole.</t>
+  </si>
+  <si>
+    <t>All pirates hold one bottle together.</t>
+  </si>
+  <si>
+    <t>One pirate ate any shark.</t>
+  </si>
+  <si>
+    <t>All pirates leaning a bucket.</t>
+  </si>
+  <si>
+    <t>A shark bites any fish.</t>
+  </si>
+  <si>
+    <t>A pirate catches any fish.</t>
+  </si>
+  <si>
+    <t>Every pirate fed a shark</t>
+  </si>
+  <si>
+    <t>A pirate is holding every bottle</t>
+  </si>
+  <si>
+    <t>Every shark is biting a fish</t>
+  </si>
+  <si>
+    <t>A shark attacked every pirate</t>
+  </si>
+  <si>
+    <t>Every pirate caught a fish</t>
+  </si>
+  <si>
+    <t>A pirate is holding every fishing pole</t>
+  </si>
+  <si>
+    <r>
+      <t>모든</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>해적들이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>상어에게</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>먹이를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>줬다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>해적하나가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>모든</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>병을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>들고있다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>모든</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>소녀들이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>강아지를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>쓰다듬고있다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>해적하나가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>모든</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>통에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>기대어있다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>상어가</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>모든</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>해적</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>한사람을</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>공격했다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>모든</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>해적들이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>물고기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>한마리를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>잡았다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>해적이</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>모든</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>낚시대를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val=".Apple SD Gothic NeoI"/>
+      </rPr>
+      <t>잡고있다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF454545"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>participant 2</t>
+  </si>
+  <si>
+    <t>모든 상어가 물고기를 깨물고있다</t>
+  </si>
+  <si>
+    <t>Every shark attacked a pirate</t>
+  </si>
+  <si>
+    <t>Every pirate is holding a fishing pole</t>
+  </si>
+  <si>
+    <t>Every pirate is holding a bottle</t>
+  </si>
+  <si>
+    <t>A pirate fed every shark</t>
+  </si>
+  <si>
+    <t>A shark is biting every fish</t>
+  </si>
+  <si>
+    <t>A pirate caught every fish</t>
+  </si>
+  <si>
+    <t>모든 해적이 상어 한마리를 먹였다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 어느 병이나 잡고 있다</t>
+  </si>
+  <si>
+    <t>모든 여자아이가 강아지 한마리를 쓰다듬고 있다</t>
+  </si>
+  <si>
+    <t>모든 상어가 물고기 한마리를 물고 있다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 어느 통에나 기대어 있다</t>
+  </si>
+  <si>
+    <t>상어 한마리가 어느 해적이나 공격했다</t>
+  </si>
+  <si>
+    <t>모든 해적이 물고기 한마리를 잡았다</t>
+  </si>
+  <si>
+    <t>해적 한사람이 어느 낚시대나 잡고 있다</t>
+  </si>
+  <si>
+    <t>모든 상어가 해적을 공격했다.</t>
+  </si>
+  <si>
+    <t>한 소녀가 모든 강아지를 쓰다듬는다.</t>
+  </si>
+  <si>
+    <t>모든 해적이 낚시대를 각각 들고있다.</t>
+  </si>
+  <si>
+    <t>모든 해적이 병을 각각 들고있다.</t>
+  </si>
+  <si>
+    <t>한명의 해적이 모든 상어에게 먹이를 줬다.</t>
+  </si>
+  <si>
+    <t>모든 해적이 한 술통에 기대고 있다.</t>
+  </si>
+  <si>
+    <t>상어한마리가 모든 물고기를 물고있다.</t>
+  </si>
+  <si>
+    <t>한명의 해적이 모든 물고기를 잡았다.</t>
+  </si>
+  <si>
+    <t>Every pirate fed shark</t>
+  </si>
+  <si>
+    <t>A pirate was holding any bottle</t>
+  </si>
+  <si>
+    <t>Every girl pet a dog</t>
+  </si>
+  <si>
+    <t>Every shark was biting a fish</t>
+  </si>
+  <si>
+    <t>A pirate is leaning on every bottle</t>
+  </si>
+  <si>
+    <t>A pirate is holding any fish pole</t>
+  </si>
+  <si>
+    <t>BATCH 1</t>
+  </si>
+  <si>
+    <t>BATCH 2</t>
+  </si>
+  <si>
+    <t>participant 3</t>
+  </si>
+  <si>
+    <t>participant 4</t>
+  </si>
+  <si>
+    <t>A shark attacekd every pirate</t>
+  </si>
+  <si>
+    <t>A pirate fed one of sharks</t>
+  </si>
+  <si>
+    <t>Every pirate is grabbing a bottle</t>
+  </si>
+  <si>
+    <t>Every pirate is holding a rod</t>
+  </si>
+  <si>
+    <t>A girl rubbed a puppy</t>
+  </si>
+  <si>
+    <t>Every sharks attacked a pirate</t>
+  </si>
+  <si>
+    <t>Every pirates are leaning toward a barrel</t>
+  </si>
+  <si>
+    <t>A shark is biting a fish</t>
+  </si>
+  <si>
+    <t>A pirates caught a fish</t>
+  </si>
+  <si>
+    <t>모든 상어가 한 마리 물고기를 물고 있다</t>
+  </si>
+  <si>
+    <t>한 해적이 모든 병을 잡고 있다</t>
+  </si>
+  <si>
+    <t>한 상어가 모든 해적을 공격했다</t>
+  </si>
+  <si>
+    <t>모든 소녀들이 한 마리 강아지를 두드리고 있다</t>
+  </si>
+  <si>
+    <t>모든 해적이 한 마리 상어를 먹였다</t>
+  </si>
+  <si>
+    <t>모든 해적이 물고기 한 마리를 잡았다</t>
+  </si>
+  <si>
+    <t>한 해적이 모든 낚시대를 잡고 있다</t>
+  </si>
+  <si>
+    <t>한 해적이 모든 통에 기대고 있다</t>
+  </si>
+  <si>
+    <t>해적이 상어를 먹이다</t>
+  </si>
+  <si>
+    <t>해적이 병을 들고 있다</t>
+  </si>
+  <si>
+    <t>해적이 낚시대를 잡고 있다</t>
+  </si>
+  <si>
+    <t>여자아이가 강아지를 키우다</t>
+  </si>
+  <si>
+    <t>상어가 해적을 공격했다</t>
+  </si>
+  <si>
+    <t>해적이 통에 기대어 있다</t>
+  </si>
+  <si>
+    <t>상어가 생선을 물고 있다</t>
+  </si>
+  <si>
+    <t>해적이 생선을 잡았다</t>
+  </si>
+  <si>
+    <t>One pirate is holding a bottle</t>
+  </si>
+  <si>
+    <t>Every girl pet one dog</t>
+  </si>
+  <si>
+    <t>Every pirate catched one fish</t>
+  </si>
+  <si>
+    <t>A pirate is holding every fishing hole</t>
+  </si>
+  <si>
+    <t>A pirate is leaning every barrel</t>
+  </si>
+  <si>
+    <t>participant 6</t>
+  </si>
+  <si>
+    <t>participant 5</t>
+  </si>
+  <si>
+    <t>Every girl is petting every dog</t>
+  </si>
+  <si>
+    <t>One pirate feed any sharks</t>
+  </si>
+  <si>
+    <t>All pirates are holding a bottle</t>
+  </si>
+  <si>
+    <t>All sharks attacked one pirate</t>
+  </si>
+  <si>
+    <t>A girl pat any dogs</t>
+  </si>
+  <si>
+    <t>All pirates are holding the same fishing pole</t>
+  </si>
+  <si>
+    <t>All pirates are leaning on the same barrel</t>
+  </si>
+  <si>
+    <t>One shark is biting any fish</t>
+  </si>
+  <si>
+    <t>A pirate caught any fish</t>
+  </si>
+  <si>
+    <t>모든 여자애들이 개 한마리를 쓰다듬고 있다</t>
+  </si>
+  <si>
+    <t>해적한사람이 모든 병을 들고 있다.</t>
+  </si>
+  <si>
+    <t>모든 해적이 고기 한마리를 잡았다</t>
+  </si>
+  <si>
+    <t>한 해적이 모든 낚시대를 다 잡고 있다.</t>
+  </si>
+  <si>
+    <t>모든 상어떼가 고기 한마리를 물고있다.</t>
+  </si>
+  <si>
+    <t>상어 한머리가 모든 해적을 공격했다.</t>
+  </si>
+  <si>
+    <t>해적 한사람이 모든 통에 기대고 있다.</t>
+  </si>
+  <si>
+    <t>participant 7</t>
+  </si>
+  <si>
+    <t>participant 8</t>
+  </si>
+  <si>
+    <t>All pirates hold a fishing rod</t>
+  </si>
+  <si>
+    <t>A pirate catched any fish</t>
+  </si>
+  <si>
+    <t>All pirates hold a bottle</t>
+  </si>
+  <si>
+    <t>A shark is biting any fish</t>
+  </si>
+  <si>
+    <t>Every pirates lean a tank</t>
+  </si>
+  <si>
+    <t>A girl touches any puppy</t>
+  </si>
+  <si>
+    <t>A pirate is catched by any shak</t>
+  </si>
+  <si>
+    <t>모든 해적이 상어 한 마리를 먹였다</t>
+  </si>
+  <si>
+    <t>모든 소녀들이 강아지 한 마리를 쓰다듬어 주고 았다</t>
+  </si>
+  <si>
+    <t>해적 한 사람이 모든 통에 기대있다</t>
+  </si>
+  <si>
+    <t>해적 한 사람이 모든 낚시대를 잡고 있다</t>
+  </si>
+  <si>
+    <t>모든 상어들이 물고기 한 마리를 같이 물고 있다</t>
+  </si>
+  <si>
+    <t>상어 한 마리가 모든 해적을 공격했다</t>
+  </si>
+  <si>
+    <t>모든 해적은 낚싯대를 드리우고 있다</t>
+  </si>
+  <si>
+    <t>한 해적이 모든 물고기를 잡았다</t>
+  </si>
+  <si>
+    <t>상어가 모든 물고기들을 잡아먹고 있다</t>
+  </si>
+  <si>
+    <t>모든 해적이 배럴에 기대어 있다</t>
+  </si>
+  <si>
+    <t>모든 상어가 한 해적을 공격했다</t>
+  </si>
+  <si>
+    <t>한 소녀가 모든 개를 쓰다듬는다</t>
+  </si>
+  <si>
+    <t>한 해적이 모든 상어를 먹인다</t>
+  </si>
+  <si>
+    <t>Every girl peddling a dog</t>
+  </si>
+  <si>
+    <t>A pirate is holding any fishing pole</t>
+  </si>
+  <si>
+    <t>A pirate is holding any bottle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2705,8 +3579,65 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val=".Apple SD Gothic NeoI"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2737,8 +3668,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2746,11 +3683,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2769,6 +3730,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3048,21 +4021,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="116" zoomScalePageLayoutView="116" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20:F35"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="29.5" customWidth="1"/>
     <col min="8" max="8" width="27.1640625" customWidth="1"/>
     <col min="16" max="16" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -3077,7 +4050,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3107,7 +4080,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -3137,7 +4110,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -3167,7 +4140,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -3197,7 +4170,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -3227,7 +4200,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -3257,7 +4230,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -3287,7 +4260,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17">
       <c r="A9" s="4">
         <v>4</v>
       </c>
@@ -3317,7 +4290,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -3347,7 +4320,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -3377,7 +4350,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -3407,7 +4380,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17">
       <c r="A13" s="4">
         <v>6</v>
       </c>
@@ -3437,7 +4410,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17">
       <c r="A14" s="4">
         <v>7</v>
       </c>
@@ -3467,7 +4440,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17">
       <c r="A15" s="4">
         <v>7</v>
       </c>
@@ -3497,7 +4470,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17">
       <c r="A16" s="4">
         <v>8</v>
       </c>
@@ -3527,7 +4500,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17">
       <c r="A17" s="4">
         <v>8</v>
       </c>
@@ -3557,7 +4530,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -3570,7 +4543,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17">
       <c r="A20" s="4">
         <v>1</v>
       </c>
@@ -3600,7 +4573,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17">
       <c r="A21" s="4">
         <v>1</v>
       </c>
@@ -3630,7 +4603,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17">
       <c r="A22" s="4">
         <v>2</v>
       </c>
@@ -3658,7 +4631,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17">
       <c r="A23" s="4">
         <v>2</v>
       </c>
@@ -3686,7 +4659,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17">
       <c r="A24" s="4">
         <v>3</v>
       </c>
@@ -3714,7 +4687,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17">
       <c r="A25" s="4">
         <v>3</v>
       </c>
@@ -3742,7 +4715,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17">
       <c r="A26" s="4">
         <v>4</v>
       </c>
@@ -3770,7 +4743,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17">
       <c r="A27" s="4">
         <v>4</v>
       </c>
@@ -3798,7 +4771,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17">
       <c r="A28" s="4">
         <v>5</v>
       </c>
@@ -3826,7 +4799,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17">
       <c r="A29" s="4">
         <v>5</v>
       </c>
@@ -3854,7 +4827,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17">
       <c r="A30" s="4">
         <v>6</v>
       </c>
@@ -3882,7 +4855,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17">
       <c r="A31" s="4">
         <v>6</v>
       </c>
@@ -3910,7 +4883,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17">
       <c r="A32" s="4">
         <v>7</v>
       </c>
@@ -3938,7 +4911,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17">
       <c r="A33" s="4">
         <v>7</v>
       </c>
@@ -3966,7 +4939,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17">
       <c r="A34" s="4">
         <v>8</v>
       </c>
@@ -3994,7 +4967,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17">
       <c r="A35" s="4">
         <v>8</v>
       </c>
@@ -4022,12 +4995,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="37" spans="1:17">
+      <c r="A37" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" ht="18">
       <c r="A38" s="4">
         <v>1</v>
       </c>
@@ -4055,7 +5028,7 @@
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="18">
       <c r="A39" s="4">
         <v>2</v>
       </c>
@@ -4083,7 +5056,7 @@
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="18">
       <c r="A40" s="4">
         <v>3</v>
       </c>
@@ -4111,7 +5084,7 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="18">
       <c r="A41" s="4">
         <v>4</v>
       </c>
@@ -4139,7 +5112,7 @@
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="18">
       <c r="A42" s="4">
         <v>5</v>
       </c>
@@ -4167,7 +5140,7 @@
       <c r="O42" s="10"/>
       <c r="P42" s="10"/>
     </row>
-    <row r="43" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="18">
       <c r="A43" s="4">
         <v>6</v>
       </c>
@@ -4195,7 +5168,7 @@
       <c r="O43" s="10"/>
       <c r="P43" s="10"/>
     </row>
-    <row r="44" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" ht="18">
       <c r="A44" s="4">
         <v>7</v>
       </c>
@@ -4223,7 +5196,7 @@
       <c r="O44" s="10"/>
       <c r="P44" s="10"/>
     </row>
-    <row r="45" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" ht="18">
       <c r="A45" s="4">
         <v>8</v>
       </c>
@@ -4251,7 +5224,7 @@
       <c r="O45" s="10"/>
       <c r="P45" s="10"/>
     </row>
-    <row r="46" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="18">
       <c r="A46" s="4">
         <v>9</v>
       </c>
@@ -4279,7 +5252,7 @@
       <c r="O46" s="10"/>
       <c r="P46" s="10"/>
     </row>
-    <row r="47" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" ht="18">
       <c r="A47" s="4">
         <v>10</v>
       </c>
@@ -4307,7 +5280,7 @@
       <c r="O47" s="10"/>
       <c r="P47" s="10"/>
     </row>
-    <row r="48" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="18">
       <c r="A48" s="4">
         <v>11</v>
       </c>
@@ -4335,7 +5308,7 @@
       <c r="O48" s="10"/>
       <c r="P48" s="10"/>
     </row>
-    <row r="49" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="18">
       <c r="A49" s="4">
         <v>12</v>
       </c>
@@ -4363,7 +5336,7 @@
       <c r="O49" s="10"/>
       <c r="P49" s="10"/>
     </row>
-    <row r="50" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="18">
       <c r="A50" s="4">
         <v>13</v>
       </c>
@@ -4398,19 +5371,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:Q1048576"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="16" max="16" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
@@ -4443,7 +5416,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="1" customFormat="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4479,7 +5452,7 @@
         <v>Every pirate is leaning on a barrel</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4511,7 +5484,7 @@
         <v>해적 한사람이 어느 통에나 기대어 있다</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4543,7 +5516,7 @@
         <v xml:space="preserve">모든 해적이 물고기 한마리를 잡았다 </v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4575,7 +5548,7 @@
         <v xml:space="preserve">A pirate caught every fish </v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4607,7 +5580,7 @@
         <v xml:space="preserve">Every pirate is holding a fishing pole </v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4639,7 +5612,7 @@
         <v>해적 한사람이 어느 낚시대나 잡고 있다</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4671,7 +5644,7 @@
         <v>모든 해적이 상어 한마리를 먹였다</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4703,7 +5676,7 @@
         <v xml:space="preserve">A pirate fed every shark </v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4735,7 +5708,7 @@
         <v xml:space="preserve">Every pirate is holding a bottle </v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4767,7 +5740,7 @@
         <v>해적 한사람이 어느 병이나 잡고 있다</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4799,7 +5772,7 @@
         <v>모든 상어가 물고기 한마리를 물고 있다</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4831,7 +5804,7 @@
         <v xml:space="preserve">A shark is biting every fish </v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4863,7 +5836,7 @@
         <v xml:space="preserve">Every shark attacked a pirate </v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4895,7 +5868,7 @@
         <v>상어 한마리가 어느 해적이나 공격했다</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4927,7 +5900,7 @@
         <v>모든 여자아이가 강아지 한마리를 쓰다듬고 있다</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4969,19 +5942,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>159</v>
       </c>
@@ -4992,34 +5966,34 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <f ca="1">RAND()</f>
-        <v>0.76521227631299871</v>
+        <v>0.16462436931028024</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <f ca="1">RAND()</f>
-        <v>0.17141283684666664</v>
+        <v>0.80762803368976666</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>122</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <f ca="1">RAND()</f>
-        <v>0.34675118643120706</v>
+        <v>0.60692234504987852</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>61</v>
@@ -5028,177 +6002,1092 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <f ca="1">RAND()</f>
-        <v>0.71521343014545402</v>
+        <v>0.61722302015749564</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <f ca="1">RAND()</f>
-        <v>0.55556138251956755</v>
+        <v>0.79983034515455842</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>125</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <f ca="1">RAND()</f>
-        <v>0.53675046619216615</v>
+        <v>8.4713394519537744E-3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <f ca="1">RAND()</f>
-        <v>0.25106422831822139</v>
+        <v>0.62443984798349905</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <f ca="1">RAND()</f>
-        <v>0.27805519817313562</v>
+        <v>0.98723893490013193</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <f ca="1">RAND()+1</f>
-        <v>1.2166830167436964</v>
+        <v>1.260469500297102</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <f ca="1">RAND()+1</f>
-        <v>1.9333379148574839</v>
+        <v>1.7262012223085805</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <f ca="1">RAND()+1</f>
-        <v>1.655877534880609</v>
+        <v>1.1553197880609207</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <f ca="1">RAND()+1</f>
-        <v>1.8667718039036472</v>
+        <v>1.8507982337209932</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <f ca="1">RAND()+1</f>
-        <v>1.9032961772290042</v>
+        <v>1.0586870716295662</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <f ca="1">RAND()+1</f>
-        <v>1.0398624543410073</v>
+        <v>1.194505835958223</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <f ca="1">RAND()+1</f>
-        <v>1.8670620451801321</v>
+        <v>1.249794180873625</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <f ca="1">RAND()+1</f>
-        <v>1.2253622691947732</v>
+        <v>1.2910915962606553</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D23">
+  <sortState ref="A2:C17">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.1640625" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="49" customWidth="1"/>
+    <col min="7" max="7" width="40.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="25" customFormat="1">
+      <c r="A1" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" t="s">
+        <v>189</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" t="s">
+        <v>190</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="F10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="B18" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="B21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="F21" t="s">
+        <v>190</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="B22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="F22" t="s">
+        <v>189</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="B23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="F23" t="s">
+        <v>188</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="B24" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="F24" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="F25" t="s">
+        <v>187</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="B27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="F27" t="s">
+        <v>191</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="B28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="F28" t="s">
+        <v>192</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="B29" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="B31" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="B32" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="B33" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="B34" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="B35" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="B36" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="E38" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="B39" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="F39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="B40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="F40" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="B41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="F41" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="B42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="F42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="B43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="F43" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="B44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="B45" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="F45" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="B46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="F46" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="B47" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C47" t="s">
+        <v>260</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="B48" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48" t="s">
+        <v>261</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="B49" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
+      <c r="F49" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="B50" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C50" t="s">
+        <v>262</v>
+      </c>
+      <c r="F50" s="18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="B51" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" t="s">
+        <v>263</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="B52" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C52" t="s">
+        <v>264</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="B53" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C53" t="s">
+        <v>265</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="B54" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>266</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="B57" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" t="s">
+        <v>269</v>
+      </c>
+      <c r="F57" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="G57" s="20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="B58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" t="s">
+        <v>270</v>
+      </c>
+      <c r="F58" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="G58" s="20" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="B59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" t="s">
+        <v>271</v>
+      </c>
+      <c r="F59" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="B60" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" t="s">
+        <v>272</v>
+      </c>
+      <c r="F60" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="B61" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" t="s">
+        <v>273</v>
+      </c>
+      <c r="F61" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="B62" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" t="s">
+        <v>187</v>
+      </c>
+      <c r="F62" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="G62" s="20" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="B63" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" t="s">
+        <v>274</v>
+      </c>
+      <c r="F63" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="B64" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" t="s">
+        <v>275</v>
+      </c>
+      <c r="F64" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7">
+      <c r="B65" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C65" t="s">
+        <v>276</v>
+      </c>
+      <c r="F65" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7">
+      <c r="B66" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" t="s">
+        <v>277</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7">
+      <c r="B67" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C67" t="s">
+        <v>233</v>
+      </c>
+      <c r="F67" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7">
+      <c r="B68" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>278</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7">
+      <c r="B69" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C69" t="s">
+        <v>279</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7">
+      <c r="B70" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C70" s="15"/>
+      <c r="F70" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7">
+      <c r="B71" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C71" t="s">
+        <v>281</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="B72" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C72" t="s">
+        <v>280</v>
+      </c>
+      <c r="F72" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C877447C-3EC8-BF4C-8B39-52A9F659FBFD}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added data of last two participants
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2437D57C-A723-094E-B474-DAFDE8A47B02}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{96408AC6-B1BA-BD4F-A4F3-3468B2F520D7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="460" windowWidth="28060" windowHeight="19980" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7100" yWindow="460" windowWidth="28060" windowHeight="19980" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sentences" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="325">
   <si>
     <t xml:space="preserve">sentence </t>
   </si>
@@ -3506,13 +3506,70 @@
   </si>
   <si>
     <t>해적은 모든 고기를 잡었다</t>
+  </si>
+  <si>
+    <t>A girl touch many dogs</t>
+  </si>
+  <si>
+    <t>A pirate catches every fish</t>
+  </si>
+  <si>
+    <t>A pirate feeds many sharks</t>
+  </si>
+  <si>
+    <t>A shark catches every fish</t>
+  </si>
+  <si>
+    <t>Every pirate holding a can</t>
+  </si>
+  <si>
+    <t>Every pirate holding a rod</t>
+  </si>
+  <si>
+    <t>Every pirate leans on barrel</t>
+  </si>
+  <si>
+    <t>Every shark fight a pirate</t>
+  </si>
+  <si>
+    <t>모든 소녀가 강아지를 이뻐한다</t>
+  </si>
+  <si>
+    <t xml:space="preserve">해적이 모든 병을 잡고 있다 </t>
+  </si>
+  <si>
+    <t>한 소녀가 모든 개를 쓰다듬었다</t>
+  </si>
+  <si>
+    <t>한 해적이 모든 상어를 먹였다</t>
+  </si>
+  <si>
+    <t>한 상어가 모든 물고기를 물고있다</t>
+  </si>
+  <si>
+    <t>모든 해적이 한 병을 잡고있다</t>
+  </si>
+  <si>
+    <t>모든 해적이 한 낚시대를 잡고있다</t>
+  </si>
+  <si>
+    <t>모든 해적이 한 배럴에 기대고 있다</t>
+  </si>
+  <si>
+    <t>Every pirate is holding a fish</t>
+  </si>
+  <si>
+    <t>A shark attacked any pirate</t>
+  </si>
+  <si>
+    <t>A pirate is holding a fishing pole</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3615,6 +3672,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Batang"/>
+      <family val="1"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -3684,7 +3748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3714,6 +3778,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5918,7 +5983,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C2" sqref="C2:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5940,20 +6005,20 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <f t="shared" ref="A2:A9" ca="1" si="0">RAND()</f>
-        <v>0.43682830337434797</v>
+        <f ca="1">RAND()</f>
+        <v>0.12451740543798717</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.36046392530101068</v>
+        <f ca="1">RAND()</f>
+        <v>0.38815293530026995</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>122</v>
@@ -5964,20 +6029,20 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.85015137975811228</v>
+        <f ca="1">RAND()</f>
+        <v>0.11675078508323733</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.35532248617882733</v>
+        <f ca="1">RAND()</f>
+        <v>0.20792758715157345</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>129</v>
@@ -5988,68 +6053,68 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.12114542848254584</v>
+        <f ca="1">RAND()</f>
+        <v>8.3730009929906535E-3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.28319557264945572</v>
+        <f ca="1">RAND()</f>
+        <v>0.3500334913688633</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.8036525074063725E-2</v>
+        <f ca="1">RAND()</f>
+        <v>0.45482872522577955</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.47746427578848616</v>
+        <f ca="1">RAND()</f>
+        <v>1.9606015409451949E-2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <f t="shared" ref="A10:A17" ca="1" si="1">RAND()+1</f>
-        <v>1.6166648379988549</v>
+        <f ca="1">RAND()+1</f>
+        <v>1.6814763435937403</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.165670755958633</v>
+        <f ca="1">RAND()+1</f>
+        <v>1.8963144712318512</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
@@ -6060,8 +6125,8 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.294830262496937</v>
+        <f ca="1">RAND()+1</f>
+        <v>1.8599855923841866</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -6072,67 +6137,67 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.4945193281084783</v>
+        <f ca="1">RAND()+1</f>
+        <v>1.1516060046598837</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>120</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.7731783523316045</v>
+        <f ca="1">RAND()+1</f>
+        <v>1.6243772251400728</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.8036670566989743</v>
+        <f ca="1">RAND()+1</f>
+        <v>1.4158404968071607</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.6064025938788724</v>
+        <f ca="1">RAND()+1</f>
+        <v>1.0655214136375699</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.8035935826619149</v>
+        <f ca="1">RAND()+1</f>
+        <v>1.712963921857811</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:C17">
-    <sortCondition ref="A1"/>
+    <sortCondition ref="C11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6141,10 +6206,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7101,10 +7166,233 @@
       <c r="A74" s="1" t="s">
         <v>268</v>
       </c>
+      <c r="E74" s="1" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="E75" s="1" t="s">
-        <v>267</v>
+      <c r="B75" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C75" t="s">
+        <v>306</v>
+      </c>
+      <c r="E75" s="1"/>
+      <c r="F75" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G75" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="B76" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76" t="s">
+        <v>307</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="B77" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77" t="s">
+        <v>308</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G77" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="B78" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C78" t="s">
+        <v>309</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="B79" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C79" t="s">
+        <v>310</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="B80" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C80" t="s">
+        <v>311</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G80" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7">
+      <c r="B81" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C81" t="s">
+        <v>312</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G81" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7">
+      <c r="B82" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C82" t="s">
+        <v>313</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G82" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7">
+      <c r="B83" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G83" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G84" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7">
+      <c r="B85" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G85" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7">
+      <c r="B86" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G86" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7">
+      <c r="B87" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G87" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7">
+      <c r="B88" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C88" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G88" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7">
+      <c r="B89" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G89" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7">
+      <c r="B90" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G90" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created new sheet of translations of relevant quantifiers
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{96408AC6-B1BA-BD4F-A4F3-3468B2F520D7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{39015FDF-569E-E546-A1B7-B6A5C09557CF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7100" yWindow="460" windowWidth="28060" windowHeight="19980" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10100" yWindow="460" windowWidth="28060" windowHeight="19980" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sentences" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="350">
   <si>
     <t xml:space="preserve">sentence </t>
   </si>
@@ -2844,9 +2844,6 @@
   </si>
   <si>
     <t>participant 5</t>
-  </si>
-  <si>
-    <t>Every girl is petting every dog</t>
   </si>
   <si>
     <t>One pirate feed any sharks</t>
@@ -3563,6 +3560,84 @@
   </si>
   <si>
     <t>A pirate is holding a fishing pole</t>
+  </si>
+  <si>
+    <t>motun</t>
+  </si>
+  <si>
+    <t>enu</t>
+  </si>
+  <si>
+    <t>kor, eng</t>
+  </si>
+  <si>
+    <t>eng, kor</t>
+  </si>
+  <si>
+    <t>every</t>
+  </si>
+  <si>
+    <t>everya</t>
+  </si>
+  <si>
+    <t>aevery</t>
+  </si>
+  <si>
+    <t>all-one</t>
+  </si>
+  <si>
+    <t>one-a</t>
+  </si>
+  <si>
+    <t>one-any</t>
+  </si>
+  <si>
+    <t>all-a</t>
+  </si>
+  <si>
+    <t>a-any</t>
+  </si>
+  <si>
+    <t>every-a</t>
+  </si>
+  <si>
+    <t>a-every</t>
+  </si>
+  <si>
+    <t>a-one</t>
+  </si>
+  <si>
+    <t>a-a</t>
+  </si>
+  <si>
+    <t>a-</t>
+  </si>
+  <si>
+    <t>every-one</t>
+  </si>
+  <si>
+    <t>all-the</t>
+  </si>
+  <si>
+    <t>a-many</t>
+  </si>
+  <si>
+    <t>every-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-a </t>
+  </si>
+  <si>
+    <t>everya, aevery --&gt; motun</t>
+  </si>
+  <si>
+    <t>enu --&gt; any</t>
+  </si>
+  <si>
+    <t>motun --&gt; every-a</t>
+  </si>
+  <si>
+    <t>enu --&gt; a-every</t>
   </si>
 </sst>
 </file>
@@ -3680,7 +3755,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3708,6 +3783,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3748,7 +3829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3779,6 +3860,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6005,8 +6089,8 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <f ca="1">RAND()</f>
-        <v>0.12451740543798717</v>
+        <f t="shared" ref="A2:A9" ca="1" si="0">RAND()</f>
+        <v>0.21484784434281412</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>133</v>
@@ -6017,8 +6101,8 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <f ca="1">RAND()</f>
-        <v>0.38815293530026995</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9.6629229462427135E-3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>122</v>
@@ -6029,8 +6113,8 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <f ca="1">RAND()</f>
-        <v>0.11675078508323733</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.17018597365599997</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>125</v>
@@ -6041,8 +6125,8 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <f ca="1">RAND()</f>
-        <v>0.20792758715157345</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.66336560408690692</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>129</v>
@@ -6053,8 +6137,8 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <f ca="1">RAND()</f>
-        <v>8.3730009929906535E-3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.94549902213874459</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>61</v>
@@ -6065,8 +6149,8 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <f ca="1">RAND()</f>
-        <v>0.3500334913688633</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.30639660604385688</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>57</v>
@@ -6077,8 +6161,8 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <f ca="1">RAND()</f>
-        <v>0.45482872522577955</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.98228690590272705</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>51</v>
@@ -6089,8 +6173,8 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <f ca="1">RAND()</f>
-        <v>1.9606015409451949E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.35871937318535552</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>65</v>
@@ -6101,8 +6185,8 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <f ca="1">RAND()+1</f>
-        <v>1.6814763435937403</v>
+        <f t="shared" ref="A10:A17" ca="1" si="1">RAND()+1</f>
+        <v>1.9729218389851784</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -6113,8 +6197,8 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <f ca="1">RAND()+1</f>
-        <v>1.8963144712318512</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.1650559017746152</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
@@ -6125,8 +6209,8 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <f ca="1">RAND()+1</f>
-        <v>1.8599855923841866</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7358679839394604</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -6137,8 +6221,8 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <f ca="1">RAND()+1</f>
-        <v>1.1516060046598837</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.9118169801492026</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -6149,8 +6233,8 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <f ca="1">RAND()+1</f>
-        <v>1.6243772251400728</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7395271528792358</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -6161,8 +6245,8 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <f ca="1">RAND()+1</f>
-        <v>1.4158404968071607</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.5723611996226583</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -6173,8 +6257,8 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <f ca="1">RAND()+1</f>
-        <v>1.0655214136375699</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6466118702396961</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
@@ -6185,8 +6269,8 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <f ca="1">RAND()+1</f>
-        <v>1.712963921857811</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.5602973512107499</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -6208,8 +6292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6243,7 +6327,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F3" t="s">
         <v>171</v>
@@ -6257,13 +6341,13 @@
         <v>133</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6271,13 +6355,13 @@
         <v>57</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F5" t="s">
         <v>172</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6285,13 +6369,13 @@
         <v>61</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F6" t="s">
         <v>173</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6299,13 +6383,13 @@
         <v>125</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F7" t="s">
         <v>174</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6313,13 +6397,13 @@
         <v>51</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -6327,13 +6411,13 @@
         <v>129</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F9" t="s">
         <v>175</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6341,13 +6425,13 @@
         <v>122</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F10" t="s">
         <v>176</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -6355,7 +6439,7 @@
         <v>164</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>177</v>
@@ -6369,7 +6453,7 @@
         <v>165</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>178</v>
@@ -6383,7 +6467,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>179</v>
@@ -6397,7 +6481,7 @@
         <v>166</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>180</v>
@@ -6411,7 +6495,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>181</v>
@@ -6425,7 +6509,7 @@
         <v>167</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>182</v>
@@ -6439,7 +6523,7 @@
         <v>168</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>183</v>
@@ -6453,7 +6537,7 @@
         <v>169</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>184</v>
@@ -6711,13 +6795,13 @@
         <v>125</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F39" t="s">
         <v>174</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -6725,13 +6809,13 @@
         <v>61</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F40" t="s">
         <v>173</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -6739,13 +6823,13 @@
         <v>65</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F41" t="s">
         <v>171</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -6753,13 +6837,13 @@
         <v>133</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F42" t="s">
         <v>17</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -6767,13 +6851,13 @@
         <v>57</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F43" t="s">
         <v>172</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -6781,13 +6865,13 @@
         <v>51</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F44" t="s">
         <v>1</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -6795,13 +6879,13 @@
         <v>129</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F45" t="s">
         <v>175</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -6809,27 +6893,27 @@
         <v>122</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F46" t="s">
         <v>176</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="B47" s="7" t="s">
-        <v>226</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F47" s="18" t="s">
         <v>179</v>
       </c>
       <c r="G47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -6837,13 +6921,13 @@
         <v>165</v>
       </c>
       <c r="C48" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F48" s="18" t="s">
         <v>178</v>
       </c>
       <c r="G48" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -6865,7 +6949,7 @@
         <v>168</v>
       </c>
       <c r="C50" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F50" s="17" t="s">
         <v>183</v>
@@ -6879,13 +6963,13 @@
         <v>169</v>
       </c>
       <c r="C51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>184</v>
       </c>
       <c r="G51" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -6893,7 +6977,7 @@
         <v>166</v>
       </c>
       <c r="C52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F52" s="18" t="s">
         <v>180</v>
@@ -6907,13 +6991,13 @@
         <v>167</v>
       </c>
       <c r="C53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F53" s="18" t="s">
         <v>182</v>
       </c>
       <c r="G53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -6921,21 +7005,21 @@
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F54" s="18" t="s">
         <v>181</v>
       </c>
       <c r="G54" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -6943,13 +7027,13 @@
         <v>57</v>
       </c>
       <c r="C57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F57" s="22" t="s">
         <v>172</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -6957,13 +7041,13 @@
         <v>122</v>
       </c>
       <c r="C58" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F58" s="22" t="s">
         <v>176</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -6971,13 +7055,13 @@
         <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F59" s="22" t="s">
         <v>173</v>
       </c>
       <c r="G59" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -6985,13 +7069,13 @@
         <v>129</v>
       </c>
       <c r="C60" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F60" s="22" t="s">
         <v>175</v>
       </c>
       <c r="G60" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -6999,13 +7083,13 @@
         <v>51</v>
       </c>
       <c r="C61" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F61" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -7019,7 +7103,7 @@
         <v>171</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -7027,13 +7111,13 @@
         <v>133</v>
       </c>
       <c r="C63" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F63" s="22" t="s">
         <v>17</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -7041,13 +7125,13 @@
         <v>125</v>
       </c>
       <c r="C64" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F64" s="22" t="s">
         <v>174</v>
       </c>
       <c r="G64" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -7055,7 +7139,7 @@
         <v>164</v>
       </c>
       <c r="C65" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F65" s="17" t="s">
         <v>177</v>
@@ -7069,13 +7153,13 @@
         <v>16</v>
       </c>
       <c r="C66" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F66" s="18" t="s">
         <v>179</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -7097,7 +7181,7 @@
         <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F68" s="18" t="s">
         <v>181</v>
@@ -7111,13 +7195,13 @@
         <v>169</v>
       </c>
       <c r="C69" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F69" s="18" t="s">
         <v>184</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -7125,13 +7209,13 @@
         <v>165</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F70" s="18" t="s">
         <v>178</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -7139,7 +7223,7 @@
         <v>167</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F71" s="18" t="s">
         <v>182</v>
@@ -7153,7 +7237,7 @@
         <v>166</v>
       </c>
       <c r="C72" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F72" s="18" t="s">
         <v>180</v>
@@ -7164,10 +7248,10 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -7175,14 +7259,14 @@
         <v>133</v>
       </c>
       <c r="C75" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G75" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -7190,13 +7274,13 @@
         <v>122</v>
       </c>
       <c r="C76" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G76" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -7204,13 +7288,13 @@
         <v>125</v>
       </c>
       <c r="C77" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>8</v>
       </c>
       <c r="G77" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -7218,13 +7302,13 @@
         <v>129</v>
       </c>
       <c r="C78" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G78" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -7232,13 +7316,13 @@
         <v>61</v>
       </c>
       <c r="C79" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G79" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -7246,13 +7330,13 @@
         <v>57</v>
       </c>
       <c r="C80" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G80" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="81" spans="2:7">
@@ -7260,13 +7344,13 @@
         <v>51</v>
       </c>
       <c r="C81" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>1</v>
       </c>
       <c r="G81" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="82" spans="2:7">
@@ -7274,13 +7358,13 @@
         <v>65</v>
       </c>
       <c r="C82" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F82" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="83" spans="2:7">
@@ -7302,7 +7386,7 @@
         <v>16</v>
       </c>
       <c r="C84" s="25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>67</v>
@@ -7322,7 +7406,7 @@
         <v>55</v>
       </c>
       <c r="G85" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="86" spans="2:7">
@@ -7350,7 +7434,7 @@
         <v>131</v>
       </c>
       <c r="G87" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="88" spans="2:7">
@@ -7364,7 +7448,7 @@
         <v>123</v>
       </c>
       <c r="G88" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="89" spans="2:7">
@@ -7372,13 +7456,13 @@
         <v>10</v>
       </c>
       <c r="C89" s="25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>127</v>
       </c>
       <c r="G89" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="90" spans="2:7">
@@ -7392,7 +7476,7 @@
         <v>120</v>
       </c>
       <c r="G90" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -7403,12 +7487,1161 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C877447C-3EC8-BF4C-8B39-52A9F659FBFD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B78" sqref="A78:B78"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="24" customFormat="1">
+      <c r="A1" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B5" t="s">
+        <v>331</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B6" t="s">
+        <v>331</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>325</v>
+      </c>
+      <c r="B21" t="s">
+        <v>338</v>
+      </c>
+      <c r="E21" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E22" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E23" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>325</v>
+      </c>
+      <c r="B24" t="s">
+        <v>339</v>
+      </c>
+      <c r="E24" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E25" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>325</v>
+      </c>
+      <c r="B27" t="s">
+        <v>339</v>
+      </c>
+      <c r="E27" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>325</v>
+      </c>
+      <c r="B28" t="s">
+        <v>339</v>
+      </c>
+      <c r="E28" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E30" t="s">
+        <v>325</v>
+      </c>
+      <c r="F30" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="E39" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>324</v>
+      </c>
+      <c r="B40" t="s">
+        <v>334</v>
+      </c>
+      <c r="E40" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>324</v>
+      </c>
+      <c r="B41" t="s">
+        <v>331</v>
+      </c>
+      <c r="E41" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>325</v>
+      </c>
+      <c r="B42" t="s">
+        <v>335</v>
+      </c>
+      <c r="E42" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>324</v>
+      </c>
+      <c r="B43" t="s">
+        <v>342</v>
+      </c>
+      <c r="E43" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>324</v>
+      </c>
+      <c r="B44" t="s">
+        <v>342</v>
+      </c>
+      <c r="E44" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="E45" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F47" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E48" t="s">
+        <v>325</v>
+      </c>
+      <c r="F48" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E50" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E51" t="s">
+        <v>325</v>
+      </c>
+      <c r="F51" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E53" t="s">
+        <v>325</v>
+      </c>
+      <c r="F53" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E54" t="s">
+        <v>325</v>
+      </c>
+      <c r="F54" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>324</v>
+      </c>
+      <c r="B57" t="s">
+        <v>334</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>324</v>
+      </c>
+      <c r="B59" t="s">
+        <v>334</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B62" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F65" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E66" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F66" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E67" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F67" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E69" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="F69" s="26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E70" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="F70" s="26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="F71" s="13" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E72" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F72" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>325</v>
+      </c>
+      <c r="B75" t="s">
+        <v>343</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="B76" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>325</v>
+      </c>
+      <c r="B77" t="s">
+        <v>343</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B80" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B82" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E83" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F83" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E84" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F84" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E85" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F85" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E86" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="F86" s="27" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E87" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="F87" s="26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E88" t="s">
+        <v>325</v>
+      </c>
+      <c r="F88" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E89" t="s">
+        <v>325</v>
+      </c>
+      <c r="F89" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E90" t="s">
+        <v>325</v>
+      </c>
+      <c r="F90" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created new word doc of criteria for identifying heritage speakers
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{39015FDF-569E-E546-A1B7-B6A5C09557CF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF5778F5-AC3B-E146-95AF-941F29640E27}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="460" windowWidth="28060" windowHeight="19980" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9960" yWindow="460" windowWidth="28060" windowHeight="19980" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sentences" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="351">
   <si>
     <t xml:space="preserve">sentence </t>
   </si>
@@ -3638,6 +3638,9 @@
   </si>
   <si>
     <t>enu --&gt; a-every</t>
+  </si>
+  <si>
+    <t>motun --&gt; all</t>
   </si>
 </sst>
 </file>
@@ -3755,7 +3758,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3789,6 +3792,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3829,7 +3838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3863,6 +3872,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6090,7 +6100,7 @@
     <row r="2" spans="1:3">
       <c r="A2">
         <f t="shared" ref="A2:A9" ca="1" si="0">RAND()</f>
-        <v>0.21484784434281412</v>
+        <v>0.40898352508084201</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>133</v>
@@ -6102,7 +6112,7 @@
     <row r="3" spans="1:3">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6629229462427135E-3</v>
+        <v>0.53867569113234115</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>122</v>
@@ -6114,7 +6124,7 @@
     <row r="4" spans="1:3">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17018597365599997</v>
+        <v>0.67509412869035157</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>125</v>
@@ -6126,7 +6136,7 @@
     <row r="5" spans="1:3">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66336560408690692</v>
+        <v>0.71102737358088097</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>129</v>
@@ -6138,7 +6148,7 @@
     <row r="6" spans="1:3">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94549902213874459</v>
+        <v>0.17277260822518081</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>61</v>
@@ -6150,7 +6160,7 @@
     <row r="7" spans="1:3">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30639660604385688</v>
+        <v>0.72923889886867321</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>57</v>
@@ -6162,7 +6172,7 @@
     <row r="8" spans="1:3">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98228690590272705</v>
+        <v>0.28148763933806409</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>51</v>
@@ -6174,7 +6184,7 @@
     <row r="9" spans="1:3">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35871937318535552</v>
+        <v>0.53638564871722261</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>65</v>
@@ -6186,7 +6196,7 @@
     <row r="10" spans="1:3">
       <c r="A10">
         <f t="shared" ref="A10:A17" ca="1" si="1">RAND()+1</f>
-        <v>1.9729218389851784</v>
+        <v>1.3414010191728196</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -6198,7 +6208,7 @@
     <row r="11" spans="1:3">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1650559017746152</v>
+        <v>1.3310716959600606</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
@@ -6210,7 +6220,7 @@
     <row r="12" spans="1:3">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7358679839394604</v>
+        <v>1.6171835512542001</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -6222,7 +6232,7 @@
     <row r="13" spans="1:3">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9118169801492026</v>
+        <v>1.6079027365633682</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -6234,7 +6244,7 @@
     <row r="14" spans="1:3">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7395271528792358</v>
+        <v>1.8835456659938792</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -6246,7 +6256,7 @@
     <row r="15" spans="1:3">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5723611996226583</v>
+        <v>1.8167430379739364</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -6258,7 +6268,7 @@
     <row r="16" spans="1:3">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6466118702396961</v>
+        <v>1.3610553024479546</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
@@ -6270,7 +6280,7 @@
     <row r="17" spans="1:3">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5602973512107499</v>
+        <v>1.9749183566656014</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -7489,8 +7499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C877447C-3EC8-BF4C-8B39-52A9F659FBFD}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B78" sqref="A78:B78"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7523,10 +7533,10 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>324</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>331</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -7557,10 +7567,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>324</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>331</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -7574,10 +7584,10 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>324</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>331</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -7603,12 +7613,15 @@
       <c r="F7" s="5" t="s">
         <v>324</v>
       </c>
+      <c r="H7" s="29" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>324</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8" s="29" t="s">
         <v>334</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -7986,10 +7999,10 @@
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>324</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="A40" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B40" s="29" t="s">
         <v>334</v>
       </c>
       <c r="E40" t="s">
@@ -7997,10 +8010,10 @@
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>324</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="A41" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B41" s="29" t="s">
         <v>331</v>
       </c>
       <c r="E41" t="s">
@@ -8019,10 +8032,10 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>324</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="A43" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B43" s="29" t="s">
         <v>342</v>
       </c>
       <c r="E43" t="s">
@@ -8030,10 +8043,10 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>324</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="A44" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B44" s="29" t="s">
         <v>342</v>
       </c>
       <c r="E44" t="s">
@@ -8186,10 +8199,10 @@
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>324</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="A57" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B57" s="29" t="s">
         <v>334</v>
       </c>
       <c r="E57" s="5" t="s">
@@ -8214,10 +8227,10 @@
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" t="s">
-        <v>324</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="A59" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B59" s="29" t="s">
         <v>334</v>
       </c>
       <c r="E59" s="5" t="s">

</xml_diff>

<commit_message>
renamed audio recordings adding "motun" and "enu"
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF5778F5-AC3B-E146-95AF-941F29640E27}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{91E67DE6-2D56-A942-9090-FD3A2932E9AF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="460" windowWidth="28060" windowHeight="19980" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16760" yWindow="460" windowWidth="28060" windowHeight="19980" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sentences" sheetId="1" r:id="rId1"/>
@@ -6100,7 +6100,7 @@
     <row r="2" spans="1:3">
       <c r="A2">
         <f t="shared" ref="A2:A9" ca="1" si="0">RAND()</f>
-        <v>0.40898352508084201</v>
+        <v>0.83171670995104929</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>133</v>
@@ -6112,7 +6112,7 @@
     <row r="3" spans="1:3">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53867569113234115</v>
+        <v>0.11811119012654525</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>122</v>
@@ -6124,7 +6124,7 @@
     <row r="4" spans="1:3">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67509412869035157</v>
+        <v>7.5301320254799853E-2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>125</v>
@@ -6136,7 +6136,7 @@
     <row r="5" spans="1:3">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71102737358088097</v>
+        <v>0.29055393901435911</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>129</v>
@@ -6148,7 +6148,7 @@
     <row r="6" spans="1:3">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17277260822518081</v>
+        <v>0.53960430766863376</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>61</v>
@@ -6160,7 +6160,7 @@
     <row r="7" spans="1:3">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72923889886867321</v>
+        <v>0.11916270726178868</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>57</v>
@@ -6172,7 +6172,7 @@
     <row r="8" spans="1:3">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28148763933806409</v>
+        <v>0.31198580354769212</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>51</v>
@@ -6184,7 +6184,7 @@
     <row r="9" spans="1:3">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53638564871722261</v>
+        <v>8.7284959880461144E-2</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>65</v>
@@ -6196,7 +6196,7 @@
     <row r="10" spans="1:3">
       <c r="A10">
         <f t="shared" ref="A10:A17" ca="1" si="1">RAND()+1</f>
-        <v>1.3414010191728196</v>
+        <v>1.9862201873877834</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -6208,7 +6208,7 @@
     <row r="11" spans="1:3">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3310716959600606</v>
+        <v>1.5574033115538197</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
@@ -6220,7 +6220,7 @@
     <row r="12" spans="1:3">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6171835512542001</v>
+        <v>1.4372742715039593</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -6232,7 +6232,7 @@
     <row r="13" spans="1:3">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6079027365633682</v>
+        <v>1.762106427339116</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -6244,7 +6244,7 @@
     <row r="14" spans="1:3">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8835456659938792</v>
+        <v>1.6411030860394478</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -6256,7 +6256,7 @@
     <row r="15" spans="1:3">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8167430379739364</v>
+        <v>1.0190172830110007</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -6268,7 +6268,7 @@
     <row r="16" spans="1:3">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3610553024479546</v>
+        <v>1.2158939961713038</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
@@ -6280,7 +6280,7 @@
     <row r="17" spans="1:3">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9749183566656014</v>
+        <v>1.9936321034548365</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -7499,8 +7499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C877447C-3EC8-BF4C-8B39-52A9F659FBFD}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Revert "renamed audio recordings adding "motun" and "enu""
This reverts commit 59183f8487ad2f3145628c944dc4f8a366819901.
</commit_message>
<xml_diff>
--- a/experiments/experigen/english-sentences.xlsx
+++ b/experiments/experigen/english-sentences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yurijo/Desktop/korean-scope/experiments/experigen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{91E67DE6-2D56-A942-9090-FD3A2932E9AF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CF5778F5-AC3B-E146-95AF-941F29640E27}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16760" yWindow="460" windowWidth="28060" windowHeight="19980" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9960" yWindow="460" windowWidth="28060" windowHeight="19980" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sentences" sheetId="1" r:id="rId1"/>
@@ -6100,7 +6100,7 @@
     <row r="2" spans="1:3">
       <c r="A2">
         <f t="shared" ref="A2:A9" ca="1" si="0">RAND()</f>
-        <v>0.83171670995104929</v>
+        <v>0.40898352508084201</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>133</v>
@@ -6112,7 +6112,7 @@
     <row r="3" spans="1:3">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11811119012654525</v>
+        <v>0.53867569113234115</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>122</v>
@@ -6124,7 +6124,7 @@
     <row r="4" spans="1:3">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5301320254799853E-2</v>
+        <v>0.67509412869035157</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>125</v>
@@ -6136,7 +6136,7 @@
     <row r="5" spans="1:3">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29055393901435911</v>
+        <v>0.71102737358088097</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>129</v>
@@ -6148,7 +6148,7 @@
     <row r="6" spans="1:3">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53960430766863376</v>
+        <v>0.17277260822518081</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>61</v>
@@ -6160,7 +6160,7 @@
     <row r="7" spans="1:3">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11916270726178868</v>
+        <v>0.72923889886867321</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>57</v>
@@ -6172,7 +6172,7 @@
     <row r="8" spans="1:3">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31198580354769212</v>
+        <v>0.28148763933806409</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>51</v>
@@ -6184,7 +6184,7 @@
     <row r="9" spans="1:3">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7284959880461144E-2</v>
+        <v>0.53638564871722261</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>65</v>
@@ -6196,7 +6196,7 @@
     <row r="10" spans="1:3">
       <c r="A10">
         <f t="shared" ref="A10:A17" ca="1" si="1">RAND()+1</f>
-        <v>1.9862201873877834</v>
+        <v>1.3414010191728196</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -6208,7 +6208,7 @@
     <row r="11" spans="1:3">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5574033115538197</v>
+        <v>1.3310716959600606</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
@@ -6220,7 +6220,7 @@
     <row r="12" spans="1:3">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4372742715039593</v>
+        <v>1.6171835512542001</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -6232,7 +6232,7 @@
     <row r="13" spans="1:3">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.762106427339116</v>
+        <v>1.6079027365633682</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -6244,7 +6244,7 @@
     <row r="14" spans="1:3">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6411030860394478</v>
+        <v>1.8835456659938792</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -6256,7 +6256,7 @@
     <row r="15" spans="1:3">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0190172830110007</v>
+        <v>1.8167430379739364</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -6268,7 +6268,7 @@
     <row r="16" spans="1:3">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2158939961713038</v>
+        <v>1.3610553024479546</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
@@ -6280,7 +6280,7 @@
     <row r="17" spans="1:3">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9936321034548365</v>
+        <v>1.9749183566656014</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -7499,8 +7499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C877447C-3EC8-BF4C-8B39-52A9F659FBFD}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>